<commit_message>
correcao do faturamento diario por lojas
</commit_message>
<xml_diff>
--- a/dados/BIBI/Dados_BIBI_PF/faturamento_diario_lojas.xlsx
+++ b/dados/BIBI/Dados_BIBI_PF/faturamento_diario_lojas.xlsx
@@ -591,13 +591,13 @@
         <v>0</v>
       </c>
       <c r="AE2">
-        <v>0</v>
+        <v>16623.32</v>
       </c>
       <c r="AF2">
         <v>0</v>
       </c>
       <c r="AG2">
-        <v>284807.17</v>
+        <v>301430.49</v>
       </c>
     </row>
     <row r="3" spans="1:33">
@@ -692,13 +692,13 @@
         <v>0</v>
       </c>
       <c r="AE3">
-        <v>0</v>
+        <v>4728.9</v>
       </c>
       <c r="AF3">
         <v>0</v>
       </c>
       <c r="AG3">
-        <v>149960.99</v>
+        <v>154689.89</v>
       </c>
     </row>
     <row r="4" spans="1:33">
@@ -793,13 +793,13 @@
         <v>4540.8</v>
       </c>
       <c r="AE4">
-        <v>0</v>
+        <v>1399</v>
       </c>
       <c r="AF4">
         <v>0</v>
       </c>
       <c r="AG4">
-        <v>88280.71000000001</v>
+        <v>89679.71000000001</v>
       </c>
     </row>
     <row r="5" spans="1:33">
@@ -894,13 +894,13 @@
         <v>1589</v>
       </c>
       <c r="AE5">
-        <v>0</v>
+        <v>1577.9</v>
       </c>
       <c r="AF5">
         <v>0</v>
       </c>
       <c r="AG5">
-        <v>86918.25</v>
+        <v>88496.14999999999</v>
       </c>
     </row>
     <row r="6" spans="1:33">
@@ -995,13 +995,13 @@
         <v>6129.8</v>
       </c>
       <c r="AE6">
-        <v>0</v>
+        <v>24329.12</v>
       </c>
       <c r="AF6">
         <v>0</v>
       </c>
       <c r="AG6">
-        <v>609967.12</v>
+        <v>634296.24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>